<commit_message>
21.01.2019 Improved enemy AI.
</commit_message>
<xml_diff>
--- a/Worked Hours.xlsx
+++ b/Worked Hours.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5279E19A-3B5A-4C5F-8BE3-066832156DBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EC91F9-D881-4454-BC23-F0A00B58FC57}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Total hours:</t>
+  </si>
+  <si>
+    <t>21.01.2019</t>
+  </si>
+  <si>
+    <t>Improved enemy AI.</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,7 +400,7 @@
       </c>
       <c r="B1" s="1">
         <f>SUM(B3:B999)</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -429,6 +435,17 @@
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enemy fights back now.
</commit_message>
<xml_diff>
--- a/Worked Hours.xlsx
+++ b/Worked Hours.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6586600A-CDF7-454A-982D-83A81330A67C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -79,12 +80,15 @@
   </si>
   <si>
     <t>Enemy AI improvements.</t>
+  </si>
+  <si>
+    <t>Enemy fights back now yay. It's almost a game.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +140,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,11 +417,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +436,7 @@
       </c>
       <c r="B1" s="1">
         <f>SUM(B3:B999)</f>
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -522,6 +526,17 @@
       </c>
       <c r="C9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New fonts, gameplay improvements.
</commit_message>
<xml_diff>
--- a/Worked Hours.xlsx
+++ b/Worked Hours.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E238959-01A1-4F92-ACB7-C48C7BF47EB3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79AFE15-CA58-4678-9C91-8B303C58AE17}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4500" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Gameplay improvements</t>
+  </si>
+  <si>
+    <t>30.01.2019</t>
+  </si>
+  <si>
+    <t>More gameplay improvements</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +448,7 @@
       </c>
       <c r="B1" s="1">
         <f>SUM(B3:B999)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -554,6 +560,17 @@
       </c>
       <c r="C11" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>